<commit_message>
ignore temp msft files
</commit_message>
<xml_diff>
--- a/docs/calculations.xlsx
+++ b/docs/calculations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Google Drive/UST/research/covg/pcb_design/kicad/covg_clamp/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Google Drive/UST/research/covg/pcb_design/kicad/covg_daq_v2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D6EEAA-ABBB-0F4A-9DF5-4E7FB93D1E14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA5617F-B32B-F040-95F8-52B19B1BED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39780" yWindow="460" windowWidth="19500" windowHeight="18360" xr2:uid="{C171766E-4946-5D44-8767-39EC626206FF}"/>
+    <workbookView xWindow="-32220" yWindow="460" windowWidth="19500" windowHeight="18360" xr2:uid="{C171766E-4946-5D44-8767-39EC626206FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="dac80508_bipolar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t xml:space="preserve">Inputs </t>
   </si>
@@ -42,15 +42,6 @@
     <t>VDAC</t>
   </si>
   <si>
-    <t>RFB</t>
-  </si>
-  <si>
-    <t>RG1</t>
-  </si>
-  <si>
-    <t>RG2</t>
-  </si>
-  <si>
     <t>VREF</t>
   </si>
   <si>
@@ -69,7 +60,22 @@
     <t>This is my design</t>
   </si>
   <si>
-    <t>eev</t>
+    <t>see Figure 78 and equation 4 of DACx0508 datasheet</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RC0603FR-07240RL</t>
+  </si>
+  <si>
+    <t>Vstep per code</t>
   </si>
 </sst>
 </file>
@@ -431,127 +437,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD118E8-0D6E-B14A-898A-2C2D942B6D21}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>33000</v>
+        <v>30000</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2">
         <f>(1 + B$2/B$3 + B$2/B$4)*B6-B$2/B$3*B$5</f>
         <v>-10</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I2" s="2">
         <f>(1 + G$2/G$3 + G$2/G$4)*G6-G$2/G$3*G$5</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-3.75</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2">
+        <f>(I3-I2)/2^16</f>
+        <v>1.1444091796875E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>8250</v>
+        <v>7500</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
         <f>(1 + B$2/B$3 + B$2/B$4)*B7-B$2/B$3*B$5</f>
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G3" s="2">
-        <v>33000</v>
+        <v>10000</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2">
         <f>(1 + G$2/G$3 + G$2/G$4)*G7-G$2/G$3*G$5</f>
-        <v>0.99999999999999978</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>11000</v>
+        <v>10000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <f>(1 + B$2/B$3 + B$2/B$4)*B8-B$2/B$3*B$5</f>
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2">
-        <v>27500</v>
+        <v>30000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2">
         <f>(1 + G$2/G$3 + G$2/G$4)*G8-G$2/G$3*G$5</f>
-        <v>2.9999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
         <v>2.5</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -565,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -576,10 +592,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -590,12 +606,17 @@
         <v>1</v>
       </c>
       <c r="G8" s="2">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G9" t="s">
-        <v>11</v>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>